<commit_message>
renamed the top scrapy folder to make it more descriptive
</commit_message>
<xml_diff>
--- a/data/2019_03_28.xlsx
+++ b/data/2019_03_28.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:AH4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,51 @@
           <t>13:17</t>
         </is>
       </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>13:18</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>13:19</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>13:20</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>13:24</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>13:25</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>13:26</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>13:27</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>13:29</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>13:31</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -606,6 +651,51 @@
           <t>75.99</t>
         </is>
       </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>75.99</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>75.99</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>75.86</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>75.86</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>75.98</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>75.98</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>75.98</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>75.98</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>75.90</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -733,6 +823,51 @@
           <t>306.00</t>
         </is>
       </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>306.00</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -858,6 +993,51 @@
       <c r="Y4" t="inlineStr">
         <is>
           <t>147.35</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>147.35</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>147.35</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>147.26</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>147.26</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>147.25</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>147.25</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>147.25</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>147.25</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>147.02</t>
         </is>
       </c>
     </row>

</xml_diff>